<commit_message>
More minor changes. Why does Cr reduced increase at really high values of k_fe2_o2???
</commit_message>
<xml_diff>
--- a/chrome-dithionite-tests/sensitivity/parameters_v2.xlsx
+++ b/chrome-dithionite-tests/sensitivity/parameters_v2.xlsx
@@ -171,7 +171,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+000"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -215,12 +215,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFF420E"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -272,7 +266,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,10 +296,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,7 +379,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -481,7 +471,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>13</v>
@@ -517,7 +507,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>13</v>
@@ -538,7 +528,7 @@
       </c>
       <c r="B8" s="2" t="n">
         <f aca="false">B7*B6</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">B6*D7</f>
@@ -573,7 +563,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>13</v>
@@ -594,7 +584,7 @@
       </c>
       <c r="B11" s="2" t="n">
         <f aca="false">B10*B9</f>
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">B9*D10</f>
@@ -874,7 +864,7 @@
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">LOG10(summary!B5)</f>
-        <v>-0.221848749616356</v>
+        <v>-0.301029995663981</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">LOG10(summary!D5)</f>
@@ -910,7 +900,7 @@
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">LOG10(summary!B7)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">LOG10(summary!D7)</f>
@@ -946,7 +936,7 @@
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">LOG10(summary!B10)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">LOG10(summary!D10)</f>
@@ -1044,7 +1034,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1128,13 +1118,13 @@
       </c>
       <c r="B5" s="0" t="n">
         <f aca="false">LOG10(summary!B5)</f>
-        <v>-0.221848749616356</v>
+        <v>-0.301029995663981</v>
       </c>
       <c r="C5" s="0" t="n">
         <f aca="false">B5-1</f>
-        <v>-1.22184874961636</v>
-      </c>
-      <c r="D5" s="8" t="n">
+        <v>-1.30102999566398</v>
+      </c>
+      <c r="D5" s="7" t="n">
         <f aca="false">LOG10(1)</f>
         <v>0</v>
       </c>
@@ -1161,21 +1151,21 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="str">
+      <c r="A7" s="7" t="str">
         <f aca="false">mads!A7</f>
         <v>factor_k_fe2_o2_slow</v>
       </c>
       <c r="B7" s="0" t="n">
         <f aca="false">LOG10(summary!B7)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C7" s="0" t="n">
         <f aca="false">B7-1</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">B7+1</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1197,21 +1187,21 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="str">
+      <c r="A9" s="7" t="str">
         <f aca="false">mads!A9</f>
         <v>factor_k_fe2_cr6_slow</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">LOG10(summary!B10)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C9" s="0" t="n">
         <f aca="false">B9-1</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">B9+1</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>